<commit_message>
Analysis of predicate frequency.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/zscores_Oct1.xlsx
+++ b/R_files/Rresults/zscores_Oct1.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="main record" sheetId="1" r:id="rId1"/>
+    <sheet name="working" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="558">
   <si>
     <t>Aeschylus</t>
   </si>
@@ -1670,6 +1671,24 @@
   </si>
   <si>
     <t>sWord</t>
+  </si>
+  <si>
+    <t>total preds</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>z-score</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>sWord / total preds</t>
   </si>
 </sst>
 </file>
@@ -2501,10 +2520,10 @@
   <dimension ref="A1:AOI15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="WJ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="WN1" sqref="WN1:WO15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51477,4 +51496,1029 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>27</v>
+      </c>
+      <c r="G1">
+        <v>27</v>
+      </c>
+      <c r="H1">
+        <v>306</v>
+      </c>
+      <c r="I1">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>551</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>318</v>
+      </c>
+      <c r="I2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>5.8922221665748502</v>
+      </c>
+      <c r="C3">
+        <v>1.67865891138622</v>
+      </c>
+      <c r="D3">
+        <v>1.7929583813291901</v>
+      </c>
+      <c r="E3">
+        <v>-0.66516703249762099</v>
+      </c>
+      <c r="F3">
+        <v>0.13271898632744</v>
+      </c>
+      <c r="G3">
+        <v>-1.1716964520091599</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>-1.06309691893796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4.3349182419111703</v>
+      </c>
+      <c r="C4">
+        <v>0.318342770386637</v>
+      </c>
+      <c r="D4">
+        <v>1.45193088252348</v>
+      </c>
+      <c r="E4">
+        <v>-1.0055379095597701</v>
+      </c>
+      <c r="F4">
+        <v>0.155398353241331</v>
+      </c>
+      <c r="G4">
+        <v>-1.0755820735159101</v>
+      </c>
+      <c r="H4">
+        <v>9.2775136263481394E-3</v>
+      </c>
+      <c r="I4">
+        <v>-0.72317968880037697</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2.5141394542377098</v>
+      </c>
+      <c r="C5">
+        <v>-1.2721205520484899</v>
+      </c>
+      <c r="D5">
+        <v>2.7288114601824698</v>
+      </c>
+      <c r="E5">
+        <v>0.268884134537687</v>
+      </c>
+      <c r="F5">
+        <v>0.52429509144201802</v>
+      </c>
+      <c r="G5">
+        <v>0.48778964029621602</v>
+      </c>
+      <c r="H5">
+        <v>8.6694463939231303E-2</v>
+      </c>
+      <c r="I5">
+        <v>2.11328667232877</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3.3025226266127499</v>
+      </c>
+      <c r="C6">
+        <v>-0.58346219982232606</v>
+      </c>
+      <c r="D6">
+        <v>2.6702612491174</v>
+      </c>
+      <c r="E6">
+        <v>0.210446657319037</v>
+      </c>
+      <c r="F6">
+        <v>0.46537004942550902</v>
+      </c>
+      <c r="G6">
+        <v>0.238067334880532</v>
+      </c>
+      <c r="H6">
+        <v>4.81417292509147E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.700759640057529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4.8313090418353601</v>
+      </c>
+      <c r="C7">
+        <v>0.75194369226602997</v>
+      </c>
+      <c r="D7">
+        <v>2.7530364372469598</v>
+      </c>
+      <c r="E7">
+        <v>0.29306246830586602</v>
+      </c>
+      <c r="F7">
+        <v>0.13495276653171401</v>
+      </c>
+      <c r="G7">
+        <v>-1.16222976817978</v>
+      </c>
+      <c r="H7">
+        <v>5.3981106612685598E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.914707585432042</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>3.9943306274964598</v>
+      </c>
+      <c r="C8">
+        <v>2.0837047852143201E-2</v>
+      </c>
+      <c r="D8">
+        <v>1.97139543873212</v>
+      </c>
+      <c r="E8">
+        <v>-0.48707354167556199</v>
+      </c>
+      <c r="F8">
+        <v>0.57982218786238904</v>
+      </c>
+      <c r="G8">
+        <v>0.72311156891272999</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>-1.06309691893796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>4.4785091674180899</v>
+      </c>
+      <c r="C9">
+        <v>0.44377047308142398</v>
+      </c>
+      <c r="D9">
+        <v>2.0589119326720802</v>
+      </c>
+      <c r="E9">
+        <v>-0.39972555389139303</v>
+      </c>
+      <c r="F9">
+        <v>0.96182747219717502</v>
+      </c>
+      <c r="G9">
+        <v>2.3420368512795999</v>
+      </c>
+      <c r="H9">
+        <v>3.0057108506161698E-2</v>
+      </c>
+      <c r="I9">
+        <v>3.8160323125591498E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>4.2052260218060704</v>
+      </c>
+      <c r="C10">
+        <v>0.20505568648672901</v>
+      </c>
+      <c r="D10">
+        <v>4.60853330315937</v>
+      </c>
+      <c r="E10">
+        <v>2.14498672030436</v>
+      </c>
+      <c r="F10">
+        <v>0.27964793456561599</v>
+      </c>
+      <c r="G10">
+        <v>-0.54901661283213599</v>
+      </c>
+      <c r="H10">
+        <v>1.61646204951223E-3</v>
+      </c>
+      <c r="I10">
+        <v>-1.0038716432205199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>4.3510572234268903</v>
+      </c>
+      <c r="C11">
+        <v>0.33244028642537199</v>
+      </c>
+      <c r="D11">
+        <v>4.20446100438771</v>
+      </c>
+      <c r="E11">
+        <v>1.74169243110163</v>
+      </c>
+      <c r="F11">
+        <v>0.42655427623206998</v>
+      </c>
+      <c r="G11">
+        <v>7.3567420469913297E-2</v>
+      </c>
+      <c r="H11">
+        <v>7.1262050921825498E-3</v>
+      </c>
+      <c r="I11">
+        <v>-0.80200111311260902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2.8396976158170202</v>
+      </c>
+      <c r="C12">
+        <v>-0.987743164297326</v>
+      </c>
+      <c r="D12">
+        <v>1.86082574142276</v>
+      </c>
+      <c r="E12">
+        <v>-0.59743034569131803</v>
+      </c>
+      <c r="F12">
+        <v>0.47005233572397698</v>
+      </c>
+      <c r="G12">
+        <v>0.25791070349013401</v>
+      </c>
+      <c r="H12">
+        <v>4.8459003682884298E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.71238420353995702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2.65114895515728</v>
+      </c>
+      <c r="C13">
+        <v>-1.1524417709066199</v>
+      </c>
+      <c r="D13">
+        <v>1.5579683200713901</v>
+      </c>
+      <c r="E13">
+        <v>-0.89970463879421803</v>
+      </c>
+      <c r="F13">
+        <v>0.31977392727002302</v>
+      </c>
+      <c r="G13">
+        <v>-0.378964033108392</v>
+      </c>
+      <c r="H13">
+        <v>7.43660295976798E-3</v>
+      </c>
+      <c r="I13">
+        <v>-0.79062849889293296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>5.7036498224295098</v>
+      </c>
+      <c r="C14">
+        <v>1.5139396170824799</v>
+      </c>
+      <c r="D14">
+        <v>1.46121261392324</v>
+      </c>
+      <c r="E14">
+        <v>-0.99627404940698805</v>
+      </c>
+      <c r="F14">
+        <v>0.24603140644388299</v>
+      </c>
+      <c r="G14">
+        <v>-0.69148230509720598</v>
+      </c>
+      <c r="H14">
+        <v>3.4230456548714198E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.19106690609149901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2.5174591226529501</v>
+      </c>
+      <c r="C15">
+        <v>-1.26922079789228</v>
+      </c>
+      <c r="D15">
+        <v>2.8520051854639701</v>
+      </c>
+      <c r="E15">
+        <v>0.39184065994828998</v>
+      </c>
+      <c r="F15">
+        <v>0.62309204198553103</v>
+      </c>
+      <c r="G15">
+        <v>0.90648772541345801</v>
+      </c>
+      <c r="H15">
+        <v>5.0181909421653501E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.77550945132696603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>552</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>553</v>
+      </c>
+      <c r="C19" t="s">
+        <v>554</v>
+      </c>
+      <c r="E19" t="s">
+        <v>553</v>
+      </c>
+      <c r="F19" t="s">
+        <v>554</v>
+      </c>
+      <c r="H19" t="s">
+        <v>553</v>
+      </c>
+      <c r="I19" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <f>B3+D3+F3+H3</f>
+        <v>7.8178995342314801</v>
+      </c>
+      <c r="C20">
+        <f>STANDARDIZE(B20,$B$34,4)</f>
+        <v>0.23745100993196688</v>
+      </c>
+      <c r="E20">
+        <f>D3/B20</f>
+        <v>0.22934016655989717</v>
+      </c>
+      <c r="F20">
+        <f>STANDARDIZE(E20,$E$34,$E$35)</f>
+        <v>-1.2225016087719021</v>
+      </c>
+      <c r="H20">
+        <f>F3/B20</f>
+        <v>1.6976297245355512E-2</v>
+      </c>
+      <c r="I20">
+        <f>STANDARDIZE(H20,$H$34,$H$35)</f>
+        <v>-1.2570560878798667</v>
+      </c>
+      <c r="K20">
+        <f>H3/B20</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>STANDARDIZE(K20,$K$34,$K$35)</f>
+        <v>-1.006954640813686</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <f>B4+D4+F4+H4</f>
+        <v>5.95152499130233</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C32" si="0">STANDARDIZE(B21,$B$34,4)</f>
+        <v>-0.22914262580032063</v>
+      </c>
+      <c r="E21">
+        <f>D4/B21</f>
+        <v>0.24395946999220519</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F32" si="1">STANDARDIZE(E21,$E$34,$E$35)</f>
+        <v>-1.0809327845410539</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H32" si="2">F4/B21</f>
+        <v>2.6110678098207277E-2</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ref="I21:I32" si="3">STANDARDIZE(H21,$H$34,$H$35)</f>
+        <v>-1.0050397042773636</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K32" si="4">H4/B21</f>
+        <v>1.5588464536243185E-3</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ref="L21:L32" si="5">STANDARDIZE(K21,$K$34,$K$35)</f>
+        <v>-0.66413619954650049</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <f>B5+D5+F5+H5</f>
+        <v>5.8539404698014286</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-0.253538756175546</v>
+      </c>
+      <c r="E22">
+        <f>D5/B22</f>
+        <v>0.46614950634696728</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1.0706869795742782</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>8.9562764456981678E-2</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>0.74559513280408551</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="4"/>
+        <v>1.480959097320169E-2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="5"/>
+        <v>2.2499414321982232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <f>B6+D6+F6+H6</f>
+        <v>6.4862956544065735</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-9.5449960024259761E-2</v>
+      </c>
+      <c r="E23">
+        <f>D6/B23</f>
+        <v>0.41167738743196408</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.54319578521834577</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="2"/>
+        <v>7.1746660069272675E-2</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>0.25405112232270227</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="4"/>
+        <v>7.4220682830282046E-3</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="5"/>
+        <v>0.62529199505642363</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <f>B7+D7+F7+H7</f>
+        <v>7.7732793522267185</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.22629596443077649</v>
+      </c>
+      <c r="E24">
+        <f>D7/B24</f>
+        <v>0.3541666666666663</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>-1.3720292015468828E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>1.7361111111111129E-2</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>-1.2464391232086867</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="4"/>
+        <v>6.944444444444451E-3</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="5"/>
+        <v>0.52025390135922811</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <f>B8+D8+F8+H8</f>
+        <v>6.5455482540909689</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-8.0636810103160927E-2</v>
+      </c>
+      <c r="E25">
+        <f>D8/B25</f>
+        <v>0.30118110236220436</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>-0.52681615014052541</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="2"/>
+        <v>8.858267716535434E-2</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>0.71855465148086806</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="5"/>
+        <v>-1.006954640813686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <f>B9+D9+F9+H9</f>
+        <v>7.5293056807935068</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.16530254657247356</v>
+      </c>
+      <c r="E26">
+        <f>D9/B26</f>
+        <v>0.2734530938123757</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>-0.79532563055715966</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>0.12774451097804398</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="3"/>
+        <v>1.7990245696620255</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>3.9920159680638719E-3</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="5"/>
+        <v>-0.12903835309752071</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <f>B10+D10+F10+H10</f>
+        <v>9.0950237215805689</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.55673205676923909</v>
+      </c>
+      <c r="E27">
+        <f>D10/B27</f>
+        <v>0.50670932195858864</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>1.4634557208309684</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>3.0747356260552739E-2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="3"/>
+        <v>-0.87711435485007416</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="4"/>
+        <v>1.7773038300897525E-4</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="5"/>
+        <v>-0.96786852509825017</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <f>B11+D11+F11+H11</f>
+        <v>8.9891987091388525</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.53027580365881</v>
+      </c>
+      <c r="E28">
+        <f>D11/B28</f>
+        <v>0.46772366930917347</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>1.0859306880545869</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>4.7451868629671559E-2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="3"/>
+        <v>-0.41623902406130997</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="4"/>
+        <v>7.9275198187995404E-4</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="5"/>
+        <v>-0.83261418662225961</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <f>B12+D12+F12+H12</f>
+        <v>5.2190346966466414</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-0.41226519946424278</v>
+      </c>
+      <c r="E29">
+        <f>D12/B29</f>
+        <v>0.3565459610027859</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="1"/>
+        <v>9.320060298389091E-3</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>9.0064995357474281E-2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="3"/>
+        <v>0.7594516182424017</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="4"/>
+        <v>9.2850510677808685E-3</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="5"/>
+        <v>1.0349954991389538</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <f>B13+D13+F13+H13</f>
+        <v>4.5363278054584608</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-0.58294192226128794</v>
+      </c>
+      <c r="E30">
+        <f>D13/B30</f>
+        <v>0.34344262295081984</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>-0.11756862288036238</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>7.0491803278688606E-2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="3"/>
+        <v>0.21942978614277839</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="4"/>
+        <v>1.6393442622950846E-3</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="5"/>
+        <v>-0.64643328003844047</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <f>B14+D14+F14+H14</f>
+        <v>7.4451242993453475</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.14425720121043373</v>
+      </c>
+      <c r="E31">
+        <f>D14/B31</f>
+        <v>0.19626436781609205</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="1"/>
+        <v>-1.5427974395779394</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>3.3045977011494171E-2</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="3"/>
+        <v>-0.81369570631134192</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="4"/>
+        <v>4.5977011494252812E-3</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="5"/>
+        <v>4.1627388318272512E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32">
+        <f>B15+D15+F15+H15</f>
+        <v>6.0427382595241053</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>-0.20633930874487683</v>
+      </c>
+      <c r="E32">
+        <f>D15/B32</f>
+        <v>0.47197231833910003</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="1"/>
+        <v>1.1270732945078465</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>0.10311418685121115</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="3"/>
+        <v>1.1194771199337841</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="4"/>
+        <v>8.3044982698961996E-3</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="5"/>
+        <v>0.81935425944568763</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>555</v>
+      </c>
+      <c r="B34">
+        <f>AVERAGE(B20:B32)</f>
+        <v>6.8680954945036126</v>
+      </c>
+      <c r="E34">
+        <f>AVERAGE(E20:E32)</f>
+        <v>0.35558351188837228</v>
+      </c>
+      <c r="H34">
+        <f>AVERAGE(H20:H32)</f>
+        <v>6.2538529731801462E-2</v>
+      </c>
+      <c r="K34">
+        <f>AVERAGE(K20:K32)</f>
+        <v>4.5787725566652998E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>556</v>
+      </c>
+      <c r="B35">
+        <f>_xlfn.STDEV.S(B20:B32)</f>
+        <v>1.3816087011048852</v>
+      </c>
+      <c r="E35">
+        <f>_xlfn.STDEV.S(E20:E32)</f>
+        <v>0.10326640425062211</v>
+      </c>
+      <c r="H35">
+        <f>_xlfn.STDEV.S(H20:H32)</f>
+        <v>3.6245186611593899E-2</v>
+      </c>
+      <c r="K35">
+        <f>_xlfn.STDEV.S(K20:K32)</f>
+        <v>4.5471487702418737E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>